<commit_message>
Getting a refill on my coffee. Need to check through this once more to make sure things calculated correctly and go through forage bag outliers, but I'm happy with where the data are getting.
</commit_message>
<xml_diff>
--- a/data/usda carbon nitrogen data.xlsx
+++ b/data/usda carbon nitrogen data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RyanMeyer/Documents/R Projects/2023_nrec_decomp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7930DFBE-CCD1-F44E-BE1E-AA172D68A536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4C986F-9C81-844D-8D18-21D5AC7744AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RG C&amp;N" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="666">
   <si>
     <t>d</t>
   </si>
@@ -1913,7 +1913,124 @@
     <t>T77</t>
   </si>
   <si>
-    <t>`</t>
+    <t>T21</t>
+  </si>
+  <si>
+    <t>F95</t>
+  </si>
+  <si>
+    <t>F130</t>
+  </si>
+  <si>
+    <t>F166</t>
+  </si>
+  <si>
+    <t>T99</t>
+  </si>
+  <si>
+    <t>T131</t>
+  </si>
+  <si>
+    <t>T167</t>
+  </si>
+  <si>
+    <t>F349</t>
+  </si>
+  <si>
+    <t>F37</t>
+  </si>
+  <si>
+    <t>F63</t>
+  </si>
+  <si>
+    <t>F136</t>
+  </si>
+  <si>
+    <t>T342</t>
+  </si>
+  <si>
+    <t>T37</t>
+  </si>
+  <si>
+    <t>T70</t>
+  </si>
+  <si>
+    <t>T142</t>
+  </si>
+  <si>
+    <t>F191</t>
+  </si>
+  <si>
+    <t>F148</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F77</t>
+  </si>
+  <si>
+    <t>T126</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>F259</t>
+  </si>
+  <si>
+    <t>F376</t>
+  </si>
+  <si>
+    <t>F20</t>
+  </si>
+  <si>
+    <t>F55</t>
+  </si>
+  <si>
+    <t>F112</t>
+  </si>
+  <si>
+    <t>F151</t>
+  </si>
+  <si>
+    <t>T278</t>
+  </si>
+  <si>
+    <t>T86</t>
+  </si>
+  <si>
+    <t>T112</t>
+  </si>
+  <si>
+    <t>T152</t>
+  </si>
+  <si>
+    <t>F211</t>
+  </si>
+  <si>
+    <t>F305</t>
+  </si>
+  <si>
+    <t>F29</t>
+  </si>
+  <si>
+    <t>F87</t>
+  </si>
+  <si>
+    <t>F186</t>
+  </si>
+  <si>
+    <t>T218</t>
+  </si>
+  <si>
+    <t>T107</t>
+  </si>
+  <si>
+    <t>T20</t>
+  </si>
+  <si>
+    <t>T561</t>
   </si>
 </sst>
 </file>
@@ -2240,7 +2357,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -2355,6 +2472,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2411,14 +2537,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2775,17 +2901,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C663"/>
+  <dimension ref="A1:C695"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <pane ySplit="1" topLeftCell="A649" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F691" sqref="F691"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" style="3"/>
-    <col min="2" max="2" width="8.6640625" style="1"/>
+    <col min="2" max="2" width="9.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" style="2"/>
+    <col min="4" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -9993,46 +10121,445 @@
         <v>38.6</v>
       </c>
     </row>
-    <row r="656" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A656" s="3" t="s">
+    <row r="656" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A656" s="4" t="s">
         <v>619</v>
       </c>
-      <c r="B656" s="1">
+      <c r="B656" s="5">
         <v>3.56</v>
       </c>
-      <c r="C656" s="2">
+      <c r="C656" s="6">
         <v>44.3</v>
       </c>
     </row>
+    <row r="657" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A657" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="B657" s="1">
+        <v>2.5274999999999999</v>
+      </c>
+      <c r="C657" s="2">
+        <v>41.9</v>
+      </c>
+    </row>
     <row r="658" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A658" s="5"/>
-      <c r="B658" s="4"/>
-      <c r="C658" s="6"/>
+      <c r="A658" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="B658" s="1">
+        <v>2.5274999999999999</v>
+      </c>
+      <c r="C658" s="2">
+        <v>41.9</v>
+      </c>
     </row>
     <row r="659" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A659" s="5"/>
-      <c r="B659" s="4"/>
-      <c r="C659" s="6"/>
+      <c r="A659" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="B659" s="1">
+        <v>2.5274999999999999</v>
+      </c>
+      <c r="C659" s="2">
+        <v>41.9</v>
+      </c>
     </row>
     <row r="660" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A660" s="5"/>
-      <c r="B660" s="4"/>
-      <c r="C660" s="6"/>
+      <c r="A660" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="B660" s="1">
+        <v>4.18</v>
+      </c>
+      <c r="C660" s="2">
+        <v>49.024999999999999</v>
+      </c>
     </row>
     <row r="661" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A661" s="5"/>
-      <c r="B661" s="4"/>
-      <c r="C661" s="6"/>
+      <c r="A661" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="B661" s="1">
+        <v>4.18</v>
+      </c>
+      <c r="C661" s="2">
+        <v>49.024999999999999</v>
+      </c>
     </row>
     <row r="662" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A662" s="5"/>
-      <c r="B662" s="4"/>
-      <c r="C662" s="6"/>
+      <c r="A662" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="B662" s="1">
+        <v>4.18</v>
+      </c>
+      <c r="C662" s="2">
+        <v>49.024999999999999</v>
+      </c>
     </row>
     <row r="663" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A663" s="5"/>
-      <c r="B663" s="4"/>
-      <c r="C663" s="6"/>
+      <c r="A663" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="B663" s="1">
+        <v>1.9650000000000001</v>
+      </c>
+      <c r="C663" s="2">
+        <v>42.524999999999999</v>
+      </c>
+    </row>
+    <row r="664" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A664" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="B664" s="1">
+        <v>1.9650000000000001</v>
+      </c>
+      <c r="C664" s="2">
+        <v>42.524999999999999</v>
+      </c>
+    </row>
+    <row r="665" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A665" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="B665" s="1">
+        <v>1.9650000000000001</v>
+      </c>
+      <c r="C665" s="2">
+        <v>42.524999999999999</v>
+      </c>
+    </row>
+    <row r="666" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A666" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="B666" s="1">
+        <v>1.9650000000000001</v>
+      </c>
+      <c r="C666" s="2">
+        <v>42.524999999999999</v>
+      </c>
+    </row>
+    <row r="667" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A667" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="B667" s="1">
+        <v>3.4849999999999999</v>
+      </c>
+      <c r="C667" s="2">
+        <v>46.825000000000003</v>
+      </c>
+    </row>
+    <row r="668" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A668" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="B668" s="1">
+        <v>3.4849999999999999</v>
+      </c>
+      <c r="C668" s="2">
+        <v>46.825000000000003</v>
+      </c>
+    </row>
+    <row r="669" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A669" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="B669" s="1">
+        <v>3.4849999999999999</v>
+      </c>
+      <c r="C669" s="2">
+        <v>46.825000000000003</v>
+      </c>
+    </row>
+    <row r="670" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A670" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="B670" s="1">
+        <v>3.4849999999999999</v>
+      </c>
+      <c r="C670" s="2">
+        <v>46.825000000000003</v>
+      </c>
+    </row>
+    <row r="671" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A671" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="B671" s="1">
+        <v>4.25</v>
+      </c>
+      <c r="C671" s="2">
+        <v>44.9</v>
+      </c>
+    </row>
+    <row r="672" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A672" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B672" s="1">
+        <v>4.25</v>
+      </c>
+      <c r="C672" s="2">
+        <v>44.9</v>
+      </c>
+    </row>
+    <row r="673" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A673" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="B673" s="1">
+        <v>4.25</v>
+      </c>
+      <c r="C673" s="2">
+        <v>44.9</v>
+      </c>
+    </row>
+    <row r="674" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A674" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="B674" s="1">
+        <v>4.25</v>
+      </c>
+      <c r="C674" s="2">
+        <v>44.9</v>
+      </c>
+    </row>
+    <row r="675" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A675" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="B675" s="1">
+        <v>3.6074999999999999</v>
+      </c>
+      <c r="C675" s="2">
+        <v>47.375</v>
+      </c>
+    </row>
+    <row r="676" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A676" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="B676" s="1">
+        <v>3.6074999999999999</v>
+      </c>
+      <c r="C676" s="2">
+        <v>47.375</v>
+      </c>
+    </row>
+    <row r="677" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A677" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="B677" s="1">
+        <v>2.665</v>
+      </c>
+      <c r="C677" s="2">
+        <v>43.15</v>
+      </c>
+    </row>
+    <row r="678" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A678" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="B678" s="1">
+        <v>2.665</v>
+      </c>
+      <c r="C678" s="2">
+        <v>43.15</v>
+      </c>
+    </row>
+    <row r="679" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A679" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="B679" s="1">
+        <v>2.665</v>
+      </c>
+      <c r="C679" s="2">
+        <v>43.15</v>
+      </c>
+    </row>
+    <row r="680" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A680" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="B680" s="1">
+        <v>2.665</v>
+      </c>
+      <c r="C680" s="2">
+        <v>43.15</v>
+      </c>
+    </row>
+    <row r="681" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A681" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="B681" s="1">
+        <v>2.665</v>
+      </c>
+      <c r="C681" s="2">
+        <v>43.15</v>
+      </c>
+    </row>
+    <row r="682" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A682" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="B682" s="1">
+        <v>2.665</v>
+      </c>
+      <c r="C682" s="2">
+        <v>43.15</v>
+      </c>
+    </row>
+    <row r="683" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A683" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="B683" s="1">
+        <v>3.97</v>
+      </c>
+      <c r="C683" s="2">
+        <v>46.8</v>
+      </c>
+    </row>
+    <row r="684" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A684" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="B684" s="1">
+        <v>3.97</v>
+      </c>
+      <c r="C684" s="2">
+        <v>46.8</v>
+      </c>
+    </row>
+    <row r="685" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A685" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="B685" s="1">
+        <v>3.97</v>
+      </c>
+      <c r="C685" s="2">
+        <v>46.8</v>
+      </c>
+    </row>
+    <row r="686" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A686" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="B686" s="1">
+        <v>3.97</v>
+      </c>
+      <c r="C686" s="2">
+        <v>46.8</v>
+      </c>
+    </row>
+    <row r="687" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A687" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="B687" s="1">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="C687" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="688" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A688" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="B688" s="1">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="C688" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="689" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A689" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="B689" s="1">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="C689" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="690" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A690" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="B690" s="1">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="C690" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="691" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A691" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="B691" s="1">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="C691" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="692" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A692" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="B692" s="1">
+        <v>4.1230000000000002</v>
+      </c>
+      <c r="C692" s="2">
+        <v>47.93</v>
+      </c>
+    </row>
+    <row r="693" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A693" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="B693" s="1">
+        <v>4.1230000000000002</v>
+      </c>
+      <c r="C693" s="2">
+        <v>47.93</v>
+      </c>
+    </row>
+    <row r="694" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A694" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="B694" s="1">
+        <v>4.1230000000000002</v>
+      </c>
+      <c r="C694" s="2">
+        <v>47.93</v>
+      </c>
+    </row>
+    <row r="695" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A695" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="B695" s="1">
+        <v>4.1230000000000002</v>
+      </c>
+      <c r="C695" s="2">
+        <v>47.93</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10041,6 +10568,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="12a57a94-3426-4524-8b8a-967e28c44898">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010057E7F401722ED14286B30E4150AB2995" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b27f0e8a88c9b2ea8d7328e121d12dff">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="12a57a94-3426-4524-8b8a-967e28c44898" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5515aa80e411e665438ee9d45cfa022" ns2:_="">
     <xsd:import namespace="12a57a94-3426-4524-8b8a-967e28c44898"/>
@@ -10224,26 +10770,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D94D4AE-9339-4823-A300-1929BA722A3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="12a57a94-3426-4524-8b8a-967e28c44898"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="12a57a94-3426-4524-8b8a-967e28c44898">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2EB9A9C6-ADCA-4A9D-9664-66F791D896DB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4388CCBA-E123-432A-A7A5-E3E12CCDD724}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10259,22 +10804,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2EB9A9C6-ADCA-4A9D-9664-66F791D896DB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D94D4AE-9339-4823-A300-1929BA722A3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="12a57a94-3426-4524-8b8a-967e28c44898"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Committing now because I'm about to make kind of an important change. In the percent N and percent C calculations we calculate the TIME 0 values for N and C using the means of ALL time points. We need to do this for just days == 0, going to try with max and min values for DAYS == 0 to see how it looks.
</commit_message>
<xml_diff>
--- a/data/usda carbon nitrogen data.xlsx
+++ b/data/usda carbon nitrogen data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RyanMeyer/Documents/R Projects/2023_nrec_decomp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4728DE6-AFBE-564E-996E-EAE2727AB26E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7887696D-0AFE-9E4D-9FAA-70A3478C9903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2913,8 +2913,8 @@
   <dimension ref="A1:C667"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A618" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D626" sqref="D626"/>
+      <pane ySplit="1" topLeftCell="A516" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B525" sqref="B525"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8683,7 +8683,7 @@
         <v>526</v>
       </c>
       <c r="B524" s="1">
-        <v>1.81</v>
+        <v>2.81</v>
       </c>
       <c r="C524" s="2">
         <v>39.700000000000003</v>
@@ -9112,10 +9112,10 @@
         <v>565</v>
       </c>
       <c r="B563" s="1">
-        <v>1.04</v>
+        <v>2.04</v>
       </c>
       <c r="C563" s="2">
-        <v>27.3</v>
+        <v>47.3</v>
       </c>
     </row>
     <row r="564" spans="1:3" x14ac:dyDescent="0.2">
@@ -10269,6 +10269,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="12a57a94-3426-4524-8b8a-967e28c44898">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010057E7F401722ED14286B30E4150AB2995" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b27f0e8a88c9b2ea8d7328e121d12dff">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="12a57a94-3426-4524-8b8a-967e28c44898" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5515aa80e411e665438ee9d45cfa022" ns2:_="">
     <xsd:import namespace="12a57a94-3426-4524-8b8a-967e28c44898"/>
@@ -10452,26 +10471,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D94D4AE-9339-4823-A300-1929BA722A3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="12a57a94-3426-4524-8b8a-967e28c44898"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="12a57a94-3426-4524-8b8a-967e28c44898">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2EB9A9C6-ADCA-4A9D-9664-66F791D896DB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4388CCBA-E123-432A-A7A5-E3E12CCDD724}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10487,22 +10505,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2EB9A9C6-ADCA-4A9D-9664-66F791D896DB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D94D4AE-9339-4823-A300-1929BA722A3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="12a57a94-3426-4524-8b8a-967e28c44898"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>